<commit_message>
Integrated chunk-based field extraction and fallback logic with Ollama (qwen3:4b)
Expanded the CAO analysis pipeline by integrating chunked text processing using the Ollama qwen3:4b model. Added support for:
	•	Field-aware prompt generation using descriptions from fields.yaml
	•	Per-chunk extraction with retry and failure threshold logic
	•	File-level fallback handling in case of repeated model failures
	•	Automatic filename injection into prompts and results
	•	MAX_JSON_FILES parameter to control batch size

Despite these improvements, Ollama continues to fail on JSON parsing and model consistency. This version sets the stage for a full migration to Gemini due to reliability concerns.
</commit_message>
<xml_diff>
--- a/inputExcel/250702 AI information matrix collapsed.xlsx
+++ b/inputExcel/250702 AI information matrix collapsed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/inputExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFCFFAC-153E-6446-9C43-598DC1FA1759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A968C3-3C0D-0A49-9062-431E53B0A75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16080" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
   <si>
     <t>CAO</t>
   </si>
@@ -227,12 +227,6 @@
     <t>training</t>
   </si>
   <si>
-    <t>pdf: start date on front page (date)</t>
-  </si>
-  <si>
-    <t>pdf: end date on front page (date)</t>
-  </si>
-  <si>
     <t>In pdf name (website: Dossier) (no or yes)</t>
   </si>
   <si>
@@ -366,6 +360,18 @@
   </si>
   <si>
     <t>salary_age_group</t>
+  </si>
+  <si>
+    <t>file name</t>
+  </si>
+  <si>
+    <t>pdf: start date usually on front page (date)</t>
+  </si>
+  <si>
+    <t>pdf: end date usually on front page (date)</t>
+  </si>
+  <si>
+    <t>pdf: search for increase, increment, ... (number in percent)</t>
   </si>
 </sst>
 </file>
@@ -818,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BF5F48-E2E4-AB45-AC3D-2386CAD72E8A}">
   <dimension ref="A1:BQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AR19" sqref="AR19"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,7 +955,7 @@
         <v>39</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AP1" s="3" t="s">
         <v>40</v>
@@ -976,7 +982,7 @@
         <v>47</v>
       </c>
       <c r="AX1" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AY1" s="4" t="s">
         <v>48</v>
@@ -991,7 +997,7 @@
         <v>51</v>
       </c>
       <c r="BC1" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="BD1" s="5" t="s">
         <v>52</v>
@@ -1000,16 +1006,16 @@
         <v>53</v>
       </c>
       <c r="BF1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="BG1" s="5" t="s">
         <v>54</v>
       </c>
       <c r="BH1" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="BI1" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="BJ1" s="5" t="s">
         <v>55</v>
@@ -1038,211 +1044,211 @@
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" t="s">
         <v>64</v>
       </c>
-      <c r="H2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>64</v>
+      </c>
+      <c r="R2" t="s">
         <v>65</v>
       </c>
-      <c r="K2" t="s">
+      <c r="S2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" t="s">
+        <v>101</v>
+      </c>
+      <c r="U2" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AM2" t="s">
         <v>99</v>
       </c>
-      <c r="L2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="AN2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP2" t="s">
         <v>66</v>
       </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="AQ2" t="s">
         <v>66</v>
       </c>
-      <c r="R2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" t="s">
-        <v>103</v>
-      </c>
-      <c r="T2" t="s">
-        <v>103</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="AR2" t="s">
         <v>66</v>
       </c>
-      <c r="V2" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" t="s">
-        <v>104</v>
-      </c>
-      <c r="X2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="AS2" t="s">
         <v>66</v>
       </c>
-      <c r="Z2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="AT2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV2" t="s">
         <v>69</v>
       </c>
-      <c r="AP2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AT2" s="7" t="s">
+      <c r="AW2" t="s">
         <v>70</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AX2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>75</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD2" t="s">
         <v>76</v>
       </c>
-      <c r="AV2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BE2" t="s">
         <v>87</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BF2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG2" t="s">
         <v>88</v>
       </c>
-      <c r="BC2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BE2" t="s">
+      <c r="BH2" t="s">
         <v>89</v>
       </c>
-      <c r="BF2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BK2" t="s">
         <v>90</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BL2" t="s">
         <v>91</v>
       </c>
-      <c r="BI2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BK2" t="s">
+      <c r="BM2" t="s">
         <v>92</v>
       </c>
-      <c r="BL2" t="s">
+      <c r="BN2" t="s">
         <v>93</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="BO2" t="s">
         <v>94</v>
       </c>
-      <c r="BN2" t="s">
+      <c r="BP2" t="s">
         <v>95</v>
       </c>
-      <c r="BO2" t="s">
+      <c r="BQ2" t="s">
         <v>96</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>97</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor: Transitioned to Gemini API and added initial prompt structure for CAO extraction
Replaced Ollama with Gemini API (gemini-2.5-pro) as Ollama performance was unreliable for structured extraction. The API is now fully integrated with retry and output-cleaning logic.
	•	Integrated Google Translate to translate extracted field values from Dutch to English to save Gemini tokens.
	•	Added fallback handling for Gemini failures and JSON parsing errors.
	•	Implemented a processing cap (MAX_JSON_FILES) and debug logging for easier testing and iteration.
	•	Field descriptions from fields.yaml are now included in Gemini prompts to guide structured JSON extraction.
	•	Preparing to drop fields.yaml and switch to a 2D matrix-style schema based on the annotated Excel templates.
	•	Next up: auto-expand ... ellipsis rows and convert the Excel-based pattern to prompt structure.
</commit_message>
<xml_diff>
--- a/inputExcel/250702 AI information matrix collapsed.xlsx
+++ b/inputExcel/250702 AI information matrix collapsed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/inputExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A968C3-3C0D-0A49-9062-431E53B0A75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B6989-C149-2543-9109-D05B49E64DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16080" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
   </bookViews>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BF5F48-E2E4-AB45-AC3D-2386CAD72E8A}">
   <dimension ref="A1:BQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,91 +865,91 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="AN1" s="2" t="s">
         <v>39</v>
@@ -1074,91 +1074,91 @@
         <v>63</v>
       </c>
       <c r="K2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
         <v>97</v>
       </c>
       <c r="M2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N2" t="s">
         <v>64</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>111</v>
-      </c>
-      <c r="O2" t="s">
-        <v>100</v>
       </c>
       <c r="P2" t="s">
         <v>100</v>
       </c>
       <c r="Q2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" t="s">
         <v>64</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>65</v>
-      </c>
-      <c r="S2" t="s">
-        <v>101</v>
       </c>
       <c r="T2" t="s">
         <v>101</v>
       </c>
       <c r="U2" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2" t="s">
         <v>64</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>65</v>
-      </c>
-      <c r="W2" t="s">
-        <v>102</v>
       </c>
       <c r="X2" t="s">
         <v>102</v>
       </c>
       <c r="Y2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>65</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>103</v>
       </c>
       <c r="AB2" t="s">
         <v>103</v>
       </c>
       <c r="AC2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD2" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>65</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>104</v>
       </c>
       <c r="AF2" t="s">
         <v>104</v>
       </c>
       <c r="AG2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH2" t="s">
         <v>64</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>65</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>105</v>
       </c>
       <c r="AJ2" t="s">
         <v>105</v>
       </c>
       <c r="AK2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL2" t="s">
         <v>64</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>65</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>99</v>
       </c>
       <c r="AN2" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Refactor LLM extraction into two-step pipeline; improve OCR logic and add runner script
	Split the LLM extraction into two steps:
	1.	Extract broadly relevant context and passages from the PDF text.
	2.	Feed that extracted subset into the structured JSON field-mapping prompt.
	•	This new architecture exists to improves precision and scalability of field extraction across CAOs.
	•	Updated small mistake in 2_extract.py.
	•	Added 5_run.py to automate the sequential execution of 2_extract.py, 3_llmExtraction.py, and 4_analysis.py using subprocess.
</commit_message>
<xml_diff>
--- a/inputExcel/250702 AI information matrix collapsed.xlsx
+++ b/inputExcel/250702 AI information matrix collapsed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzpiazolo/Documents/Python/CAOsDataExtraction/inputExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B6989-C149-2543-9109-D05B49E64DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47294F9B-45C5-CA45-819D-802F7788670F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16080" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
+    <workbookView xWindow="3180" yWindow="500" windowWidth="25600" windowHeight="16080" xr2:uid="{DE6B04FB-4535-6B4B-8490-9A662190B816}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="104">
   <si>
     <t>CAO</t>
   </si>
@@ -62,9 +62,6 @@
     <t>date_of_formal_notification</t>
   </si>
   <si>
-    <t>temporary</t>
-  </si>
-  <si>
     <t>TTW</t>
   </si>
   <si>
@@ -170,12 +167,6 @@
     <t>retire_age_plus</t>
   </si>
   <si>
-    <t>age_group</t>
-  </si>
-  <si>
-    <t>maternity_leave_weeks</t>
-  </si>
-  <si>
     <t>maternity_pay</t>
   </si>
   <si>
@@ -191,21 +182,12 @@
     <t>term_period_employer</t>
   </si>
   <si>
-    <t>term_period_employer_unit</t>
-  </si>
-  <si>
     <t>term_period_worker</t>
   </si>
   <si>
-    <t>term_period_worker_unit</t>
-  </si>
-  <si>
     <t>probation_period</t>
   </si>
   <si>
-    <t>duration_worked</t>
-  </si>
-  <si>
     <t>overtime_compensation</t>
   </si>
   <si>
@@ -227,158 +209,152 @@
     <t>training</t>
   </si>
   <si>
-    <t>In pdf name (website: Dossier) (no or yes)</t>
-  </si>
-  <si>
-    <t>pdf: hourly, monthly or yearly (or something else)</t>
-  </si>
-  <si>
-    <t>pdf: search for increase (number in percent)</t>
-  </si>
-  <si>
-    <t>pdf: search for the words “AOW”, “pension”, and “scheme.”,.. (text)</t>
-  </si>
-  <si>
-    <t>pdf: we only want to look at 21 years and olders - hence usually we should have "21 years and olders"</t>
-  </si>
-  <si>
-    <t>pdf: searched for the words “AOW”, “pension”, and “scheme.”,..  to find age (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information there is about maternity, kids and aoption leave pay (text or number, percent of original pay)</t>
-  </si>
-  <si>
-    <t>pdf: all information there is about maternity, kids and aoption, which is not included in the 2 previous columns (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information there is about vacation and holiday duration (number or text)</t>
-  </si>
-  <si>
     <t>vacation_time</t>
   </si>
   <si>
-    <t>pdf: all information there is about vacation and holiday duration unit (text: usually hours or days per year but can be something else as well)</t>
-  </si>
-  <si>
-    <t>pdf: all information there is about maternity, kids and aoption leave duration (text or number) - if its not weeks but days or hours mention it</t>
-  </si>
-  <si>
-    <t>pdf: all information there is about vacation and holiday which is not mentioned in the previous 2 columns (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information about period of contract termination of worker</t>
-  </si>
-  <si>
     <t>term_employer_note</t>
   </si>
   <si>
     <t>term_worker_note</t>
   </si>
   <si>
-    <t>probation_period_unit</t>
-  </si>
-  <si>
     <t>probation_note</t>
   </si>
   <si>
-    <t>pdf: all information about duration worked of workers - usually no information found (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information about probation of new workers not mentioned in the previous 2 columns (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information about contract termination of employer not mentioned in the previous 2 columns (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information about contract termination of worker not mentioned in the previous 2 columns (text)</t>
-  </si>
-  <si>
-    <t>pdf: all information about period of contract termination of employer (text or number)</t>
-  </si>
-  <si>
-    <t>pdf: all information about unit of period of contract termination of employer (text or number)</t>
-  </si>
-  <si>
-    <t>pdf: all information about unit of period of contract termination of worker (text or number)</t>
-  </si>
-  <si>
-    <t>pdf: all information about period of probation of new workers (text or number)</t>
-  </si>
-  <si>
-    <t>pdf: all information about unit of period of probation of new workers (text or number)</t>
-  </si>
-  <si>
-    <t>pdf: all information about overtime pay / compensation - important include unit, usually euro per hour (text)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: all information about maximum of hours allowed to work - in total or overtime but mention which one (text) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: all information about minimum of hours, days, weeks, months needed to work per day, weeks, month or year (text) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: all information about night, evening, morning or day shifts (text) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: all information about the minimum allowance of overtime (text) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: all information about the maximum allowance of overtime (text) </t>
-  </si>
-  <si>
-    <t>pdf: all information about training of workers and emplyers (text)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in first wage table (number)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pdf: what type of worker and what type of age - usually but not always next to wage table - focus on normal / basic wage type(text) </t>
-  </si>
-  <si>
-    <t>pdf: 1st jobgroup - should be mentioned in wage table as column titles (letter, number or text)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in second table (number)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in third wage table (number)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in fourth wage table (number)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in fifth table (number)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in sixth wage table (number)</t>
-  </si>
-  <si>
-    <t>pdf: 1st wage in seventh wage table (number)</t>
-  </si>
-  <si>
-    <t>leave empty</t>
+    <t>…</t>
   </si>
   <si>
     <t>salary_age_group</t>
   </si>
   <si>
-    <t>file name</t>
-  </si>
-  <si>
-    <t>pdf: start date usually on front page (date)</t>
-  </si>
-  <si>
-    <t>pdf: end date usually on front page (date)</t>
-  </si>
-  <si>
-    <t>pdf: search for increase, increment, ... (number in percent)</t>
+    <t>more_salaries</t>
+  </si>
+  <si>
+    <t>File_name</t>
+  </si>
+  <si>
+    <t>pdf file name (text).</t>
+  </si>
+  <si>
+    <t>In pdf file name. (boolean: Yes/No). Ex: Yes; No</t>
+  </si>
+  <si>
+    <t>Does the CAO file contain additional basic/normal wage tables beyond the 7 already extracted? (Boolean: Yes/No). Ex: Yes; No</t>
+  </si>
+  <si>
+    <t>All additional context related to salary interpretation not covered in other fields (text). Ex: Youth salary scales phased out from 2014; Hourly wage = monthly salary / 156; Classification via FWG® system; Introductory salary scales abolished as of 2013</t>
+  </si>
+  <si>
+    <t>Age group the salary tables apply to, considering only workers aged 21 and older (text). Ex: 21 years and older; 22 years and olders</t>
+  </si>
+  <si>
+    <t>All information related to the basic pension premium and scheme (text). Ex: 50% of the pension premium will be paid by the employee; The pension scheme follows the rules of Stichting Bedrijfstakpensioenfonds; Employees aged 21 to 68 are registered with the Food Industry Pension Fund; The RVU allows early retirement up to AOW age if certain conditions are met</t>
+  </si>
+  <si>
+    <t>Retirement age for the basic pension scheme (text or number). Ex: 67; 68; 67–68</t>
+  </si>
+  <si>
+    <t>Retirement age for the additional or “plus” pension premium scheme (text or number). Ex: 65; 68; 66–68</t>
+  </si>
+  <si>
+    <t>pension_age_group</t>
+  </si>
+  <si>
+    <t>Age group eligible for the pension scheme (text). Ex: 21 years and older; 22 years and older</t>
+  </si>
+  <si>
+    <t>All information related to additional or “plus” pension premiums, including age-related schemes like the Generation Policy and changes in contribution percentages (text). Ex: Pension premium increased to 21,4% in 2021, split evenly between employer and employee; Generation Policy applies to workers aged 60+ between 2018 and 2023; 0,2% premium increase for employees offset by wage increase on 1-6-2021</t>
+  </si>
+  <si>
+    <t>All information related to the duration of maternity, adoption, or child-related leave (text). Ex: 5 days of paid maternity leave; At least 16 weeks; Additional 4 weeks in case of multiple births; Up to 5 weeks extra within 6 months after birth</t>
+  </si>
+  <si>
+    <t>All available information about the amount of vacation or holiday time employees are entitled to (number or text). Include base and extra entitlements. Ex: 0.0769; 192; 20</t>
+  </si>
+  <si>
+    <t>maternity_leave</t>
+  </si>
+  <si>
+    <t>All available information about salary, benefits, or compensation during maternity, adoption, or child-related leave (text). Include both employer and UWV contributions. Ex: 100% paid by employer; 70% UWV benefit; 100% of maximum daily wage</t>
+  </si>
+  <si>
+    <t>All additional context related to maternity/ adoption/ child-related leave rules not covered in other fields (text). Include among other things rights, accruals, flexibility, partner substitution, and legal protections. Ex: Vacation accrues during leave; Leave may be split; Partner receives remaining leave if employee dies; 1 hour weekly reduction after birth</t>
+  </si>
+  <si>
+    <t>All additional vacation/ holiday-related information not covered in other fields (text). Include accrual rules, holiday years, age/tenure-based bonuses, payout terms, and holiday allowance rules. Ex: Holiday year runs June–May; 8% holiday allowance; 3 weeks of consecutive vacation; 5 extra days after 40 years of service</t>
+  </si>
+  <si>
+    <t>All information about the notice period duration or unit for worker-initiated contract termination (text). Include special rules based on age, start date, or contract length. Ex: 1 week if less than 2 years employed; 10 days; 6 weeks max based on age and service duration</t>
+  </si>
+  <si>
+    <t>All information about the notice period duration or unit for employer-initiated contract termination (text). Include special rules based on age, start date, or contract length. Ex: 1 month for contracts longer than 6 months; 4 weeks for employees with 10–15 years of service; Statutory period applies if longer than agreed term</t>
+  </si>
+  <si>
+    <t>Unit or accrual structure of the vacation time reported in the previous column "vacation_time" (text). Be precise about whether it’s hours, days, or a formula-based accrual. Ex: hours per vacation year; days per full-time contract</t>
+  </si>
+  <si>
+    <t>All other information about employer-initiated contract termination not covered in the previous column "term_period_employer" (text). Include legal references, conditions, exceptions, or case-specific rules. Ex: Civil Code provisions apply; Prior employment counts toward service years; Periods may be defined in months or 4-week cycles</t>
+  </si>
+  <si>
+    <t>All other information about worker-initiated contract termination not covered in the previous column "term_period_worker" (text). Include conditions, exceptions, legal references, or case-specific clauses. Ex: Old rule applies for employees aged 45+ as of Jan 1, 1999; Starting date for notice is always a Saturday</t>
+  </si>
+  <si>
+    <t>All information about the length or conditions of the probation period for new workers (text). Include all relevant rules based on contract length or type. Ex: 2 months for indefinite contracts; No trial period if contract ≤ 6 months; 1 month max for fixed-term contracts between 6 and 24 months</t>
+  </si>
+  <si>
+    <t>All other information about the probation period not covered in the previous column "probation_period" (text). Include references to conditions, exceptions, legal references, case-specific clauses or when probation is disallowed. Ex: Trial period only allowed if new role involves substantially different responsibilities; Article 7:652 of the Civil Code applies</t>
+  </si>
+  <si>
+    <t>All information about overtime pay or compensation, including units, percentages, and whether compensation is given in time or money (text). Include legal rules, employer-specific clauses, and time limits. Ex: 35% surcharge on basic hourly wage; Paid time off within 4 weeks; 100% of hourly wage plus overtime premium; Overtime after 152 hours per period</t>
+  </si>
+  <si>
+    <t>All information about the maximum allowed working hours or overtime hours, including what type of time it applies to and for which worker categories (text). Ex: 12 hours per day; Max 10 hours of overtime per week; 36 hours max overtime per 3 pay periods; 52-hour weekly average if salary exceeds IP number 74</t>
+  </si>
+  <si>
+    <t>All information about the minimum required number of hours, days, weeks, or months to be worked, including units and reference periods (text). Ex: 24 hours per week; 8 hours per day minimum; 20 working days per month</t>
+  </si>
+  <si>
+    <t>All information about shift-based work and related compensation, including night, evening, early morning, and weekend shifts (text). Include hours, pay surcharges, limitations, and scheduling rules. Ex: 25% surcharge from 8pm–10pm; 50% surcharge between 10pm–6am; Night shift defined as work between 00:00 and 06:00; Max 20 shifts per 4-week period</t>
+  </si>
+  <si>
+    <t>All information about the minimum allowance for overtime or night shift work, including duration, compensation, and applicable legal limits (text). Ex: At least 4.5-hour shift to qualify for night compensation; Minimum 1 paid break for shifts covering 00:00–06:00; 16 night shifts over 16 weeks triggers lower working hour threshold</t>
+  </si>
+  <si>
+    <t>All information about the maximum allowance for overtime or night shift work, including duration, compensation, and applicable legal limits (text). (text). Ex: Max 12 hours per day; Max 43 night shifts in 16 weeks; Max 36 overtime hours per 3 pay periods; Working time averaged over 13 weeks not to exceed 48 hours</t>
+  </si>
+  <si>
+    <t>All information related to training, development, or education for employees or employers (text). Include training rights, budgets, mandatory recognition, funding percentages, and types of courses. Ex: Minimum 2% of annual payroll must be used for training; POB budget of €175 per year; Dutch language course and vocational training; Only recognized training companies may provide internships</t>
+  </si>
+  <si>
+    <t>Wage, Pension, Leave, Termination, Overtime, Training</t>
+  </si>
+  <si>
+    <t>start date of contract usually on front page (dates). Ex: 01/04/2019; 01/01/2017; 01/07/2018</t>
+  </si>
+  <si>
+    <t>end date of contract usually on front page (dates). Ex: 31/01/2023; 31/03/2019; 28/02/2014</t>
+  </si>
+  <si>
+    <t>start dates of wage tables (dates in dd/mm/yyyy format). Ex: 01/01/2018; 01/01/2017; 01/07/2010</t>
+  </si>
+  <si>
+    <t>Units of the salary values in the wage tables. (texts). Ex: hourly; monthly</t>
+  </si>
+  <si>
+    <t>Salaries of the job groups. Usually listed in wage tables. (numbers). Ex: 13,17; 21,59; 9,58</t>
+  </si>
+  <si>
+    <t>all information about jobgroups. Often mentioned in wage tables (numbers or text). Ex: I=Statutory minimum wage (WML); F-21-5; 65-12-57</t>
+  </si>
+  <si>
+    <t>Percentage increases of salaries in wage tables. (numbers with % - may appear outside the tables, often near the Dutch words for increase such as “verhoging” or “loonsverhoging”). Ex: 1%; 3%; 10,5%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,6 +376,25 @@
       <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0E0E0E"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -440,12 +435,23 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -455,9 +461,18 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color rgb="FF000000"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -467,27 +482,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,439 +842,385 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BF5F48-E2E4-AB45-AC3D-2386CAD72E8A}">
-  <dimension ref="A1:BQ7"/>
+  <dimension ref="A1:BN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BG5" sqref="BG5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:69" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:66" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AX1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AY1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BA1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BB1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BC1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="BD1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="BE1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="BF1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="BG1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="BH1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="BI1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="BK1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN1" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" t="s">
+        <v>103</v>
+      </c>
+      <c r="W2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" t="s">
         <v>72</v>
-      </c>
-      <c r="AY1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AZ1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="BA1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="BC1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="BG1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BQ1" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L2" t="s">
-        <v>97</v>
-      </c>
-      <c r="M2" t="s">
-        <v>97</v>
-      </c>
-      <c r="N2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O2" t="s">
-        <v>111</v>
-      </c>
-      <c r="P2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>100</v>
-      </c>
-      <c r="R2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T2" t="s">
-        <v>101</v>
-      </c>
-      <c r="U2" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT2" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="AU2" t="s">
         <v>74</v>
       </c>
       <c r="AV2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="AW2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AX2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AY2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AZ2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="BA2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" t="s">
         <v>85</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BD2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE2" t="s">
         <v>86</v>
       </c>
-      <c r="BC2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>87</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>84</v>
       </c>
       <c r="BG2" t="s">
         <v>88</v>
       </c>
-      <c r="BH2" t="s">
+      <c r="BH2" s="10" t="s">
         <v>89</v>
       </c>
       <c r="BI2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="BJ2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="BK2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="BL2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="BM2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="BN2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BP2" t="s">
         <v>95</v>
       </c>
-      <c r="BQ2" t="s">
-        <v>96</v>
-      </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.2">
-      <c r="AT7" s="7"/>
+    <row r="6" spans="1:66" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="BH9" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="11" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>